<commit_message>
transform the rating attempt
</commit_message>
<xml_diff>
--- a/data/ml_perform_crossval_agg_2022-11-13.xlsx
+++ b/data/ml_perform_crossval_agg_2022-11-13.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.rahmadi\Documents\Git_code\AdamThesis\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854B5A89-017F-4DC2-B7FF-FCA0CF3435DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -67,8 +73,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +137,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -177,7 +191,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -209,9 +223,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -243,6 +275,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -418,14 +468,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +506,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -465,25 +517,25 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>0.07378598229559166</v>
+        <v>7.3785982295591662E-2</v>
       </c>
       <c r="E2">
-        <v>0.003051517171260265</v>
+        <v>3.0515171712602652E-3</v>
       </c>
       <c r="F2">
-        <v>0.07216012071966166</v>
+        <v>7.2160120719661658E-2</v>
       </c>
       <c r="G2">
-        <v>0.00897073916139569</v>
+        <v>8.9707391613956904E-3</v>
       </c>
       <c r="H2">
-        <v>0.0004309070379207606</v>
+        <v>4.3090703792076062E-4</v>
       </c>
       <c r="I2">
-        <v>0.008763336567732715</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>8.763336567732715E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -494,25 +546,25 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>0.077428773516</v>
+        <v>7.7428773515999999E-2</v>
       </c>
       <c r="E3">
-        <v>0.003732284649554552</v>
+        <v>3.7322846495545518E-3</v>
       </c>
       <c r="F3">
-        <v>0.07686424440577264</v>
+        <v>7.6864244405772636E-2</v>
       </c>
       <c r="G3">
-        <v>0.00940730602708691</v>
+        <v>9.4073060270869098E-3</v>
       </c>
       <c r="H3">
-        <v>0.0004224746908959231</v>
+        <v>4.2247469089592309E-4</v>
       </c>
       <c r="I3">
-        <v>0.009433399699594013</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>9.4333996995940132E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -523,25 +575,25 @@
         <v>23</v>
       </c>
       <c r="D4">
-        <v>0.07523830606526444</v>
+        <v>7.5238306065264438E-2</v>
       </c>
       <c r="E4">
-        <v>0.003325767642769966</v>
+        <v>3.325767642769966E-3</v>
       </c>
       <c r="F4">
-        <v>0.07384133010266797</v>
+        <v>7.3841330102667968E-2</v>
       </c>
       <c r="G4">
-        <v>0.009039501475551114</v>
+        <v>9.0395014755511142E-3</v>
       </c>
       <c r="H4">
-        <v>0.0003437603854410516</v>
+        <v>3.4376038544105161E-4</v>
       </c>
       <c r="I4">
-        <v>0.008836469753084388</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>8.8364697530843878E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -552,25 +604,25 @@
         <v>23</v>
       </c>
       <c r="D5">
-        <v>0.07621311702886625</v>
+        <v>7.6213117028866253E-2</v>
       </c>
       <c r="E5">
-        <v>0.003477949138692712</v>
+        <v>3.477949138692712E-3</v>
       </c>
       <c r="F5">
-        <v>0.0747916410319511</v>
+        <v>7.47916410319511E-2</v>
       </c>
       <c r="G5">
-        <v>0.009181294363172693</v>
+        <v>9.1812943631726929E-3</v>
       </c>
       <c r="H5">
-        <v>0.0003997834762595224</v>
+        <v>3.997834762595224E-4</v>
       </c>
       <c r="I5">
-        <v>0.009136519230493032</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>9.1365192304930318E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -581,25 +633,25 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>0.07852278787116476</v>
+        <v>7.8522787871164762E-2</v>
       </c>
       <c r="E6">
-        <v>0.005558118348145807</v>
+        <v>5.5581183481458072E-3</v>
       </c>
       <c r="F6">
-        <v>0.07754768972749286</v>
+        <v>7.7547689727492861E-2</v>
       </c>
       <c r="G6">
-        <v>0.009605253011989509</v>
+        <v>9.6052530119895094E-3</v>
       </c>
       <c r="H6">
-        <v>0.0008894848560776244</v>
+        <v>8.8948485607762444E-4</v>
       </c>
       <c r="I6">
-        <v>0.009259569694598801</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>9.2595696945988008E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -610,25 +662,25 @@
         <v>23</v>
       </c>
       <c r="D7">
-        <v>0.08551221557866424</v>
+        <v>8.5512215578664244E-2</v>
       </c>
       <c r="E7">
-        <v>0.006136179778158894</v>
+        <v>6.1361797781588944E-3</v>
       </c>
       <c r="F7">
-        <v>0.08441946584083615</v>
+        <v>8.441946584083615E-2</v>
       </c>
       <c r="G7">
-        <v>0.01167633157112464</v>
+        <v>1.167633157112464E-2</v>
       </c>
       <c r="H7">
-        <v>0.001223233827571347</v>
+        <v>1.223233827571347E-3</v>
       </c>
       <c r="I7">
-        <v>0.01163374950901253</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>1.1633749509012531E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -639,25 +691,25 @@
         <v>23</v>
       </c>
       <c r="D8">
-        <v>0.0857075601114043</v>
+        <v>8.5707560111404305E-2</v>
       </c>
       <c r="E8">
-        <v>0.009580565839792707</v>
+        <v>9.5805658397927068E-3</v>
       </c>
       <c r="F8">
-        <v>0.08339026840514829</v>
+        <v>8.3390268405148293E-2</v>
       </c>
       <c r="G8">
-        <v>0.01284386112494162</v>
+        <v>1.2843861124941619E-2</v>
       </c>
       <c r="H8">
-        <v>0.004293169460190751</v>
+        <v>4.2931694601907513E-3</v>
       </c>
       <c r="I8">
-        <v>0.01141545802879409</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>1.141545802879409E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -668,25 +720,25 @@
         <v>23</v>
       </c>
       <c r="D9">
-        <v>0.08215108695259447</v>
+        <v>8.2151086952594474E-2</v>
       </c>
       <c r="E9">
-        <v>0.005143777899296147</v>
+        <v>5.1437778992961466E-3</v>
       </c>
       <c r="F9">
-        <v>0.08102290933830258</v>
+        <v>8.1022909338302584E-2</v>
       </c>
       <c r="G9">
-        <v>0.01064285614134401</v>
+        <v>1.064285614134401E-2</v>
       </c>
       <c r="H9">
-        <v>0.0009794170733031218</v>
+        <v>9.7941707330312182E-4</v>
       </c>
       <c r="I9">
-        <v>0.01037284961291291</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>1.037284961291291E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -697,25 +749,25 @@
         <v>4</v>
       </c>
       <c r="D10">
-        <v>0.07336057565815612</v>
+        <v>7.3360575658156124E-2</v>
       </c>
       <c r="E10">
-        <v>0.003670884872980942</v>
+        <v>3.670884872980942E-3</v>
       </c>
       <c r="F10">
-        <v>0.07163597686201599</v>
+        <v>7.163597686201599E-2</v>
       </c>
       <c r="G10">
-        <v>0.008819976051658931</v>
+        <v>8.8199760516589308E-3</v>
       </c>
       <c r="H10">
-        <v>0.000484152144373442</v>
+        <v>4.8415214437344198E-4</v>
       </c>
       <c r="I10">
-        <v>0.008610939154528759</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>8.6109391545287593E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -726,25 +778,25 @@
         <v>23</v>
       </c>
       <c r="D11">
-        <v>0.08315502307190045</v>
+        <v>8.3155023071900452E-2</v>
       </c>
       <c r="E11">
-        <v>0.004425535427999435</v>
+        <v>4.4255354279994349E-3</v>
       </c>
       <c r="F11">
-        <v>0.08177044770954367</v>
+        <v>8.177044770954367E-2</v>
       </c>
       <c r="G11">
-        <v>0.01106840732776477</v>
+        <v>1.1068407327764771E-2</v>
       </c>
       <c r="H11">
-        <v>0.001000499666630714</v>
+        <v>1.0004996666307139E-3</v>
       </c>
       <c r="I11">
-        <v>0.01075609186077808</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>1.075609186077808E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -755,25 +807,25 @@
         <v>23</v>
       </c>
       <c r="D12">
-        <v>0.07884388608739663</v>
+        <v>7.8843886087396634E-2</v>
       </c>
       <c r="E12">
-        <v>0.003566291948441764</v>
+        <v>3.566291948441764E-3</v>
       </c>
       <c r="F12">
-        <v>0.07678925341985991</v>
+        <v>7.6789253419859912E-2</v>
       </c>
       <c r="G12">
-        <v>0.01007073059039915</v>
+        <v>1.007073059039915E-2</v>
       </c>
       <c r="H12">
-        <v>0.0007093622313282139</v>
+        <v>7.0936223132821391E-4</v>
       </c>
       <c r="I12">
-        <v>0.009976896317661859</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>9.9768963176618593E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -784,22 +836,22 @@
         <v>23</v>
       </c>
       <c r="D13">
-        <v>0.08050353623484616</v>
+        <v>8.0503536234846157E-2</v>
       </c>
       <c r="E13">
-        <v>0.002141159075636861</v>
+        <v>2.141159075636861E-3</v>
       </c>
       <c r="F13">
-        <v>0.08103244109023745</v>
+        <v>8.1032441090237453E-2</v>
       </c>
       <c r="G13">
-        <v>0.01033401179824038</v>
+        <v>1.0334011798240381E-2</v>
       </c>
       <c r="H13">
-        <v>0.0002733240051628365</v>
+        <v>2.7332400516283649E-4</v>
       </c>
       <c r="I13">
-        <v>0.01041625367904648</v>
+        <v>1.0416253679046481E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>